<commit_message>
adding diet records from Howell 1924
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_Howell_1924_GN.xlsx
+++ b/AvianDietDatabase_Howell_1924_GN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>Common_Name</t>
   </si>
@@ -168,6 +168,165 @@
   </si>
   <si>
     <t>Alabama</t>
+  </si>
+  <si>
+    <t>Pied-billed Grebe</t>
+  </si>
+  <si>
+    <t>Podilymbus podiceps</t>
+  </si>
+  <si>
+    <t>Common Loon</t>
+  </si>
+  <si>
+    <t>Gavia immer</t>
+  </si>
+  <si>
+    <t>Gaviidae</t>
+  </si>
+  <si>
+    <t>European Herring Gull</t>
+  </si>
+  <si>
+    <t>Larus argentatus</t>
+  </si>
+  <si>
+    <t>Laridae</t>
+  </si>
+  <si>
+    <t>Ring-billed Gull</t>
+  </si>
+  <si>
+    <t>Larus delawarensis</t>
+  </si>
+  <si>
+    <t>Laughing Gull</t>
+  </si>
+  <si>
+    <t>Leucophaeus atricilla</t>
+  </si>
+  <si>
+    <t>Bonaparte's Gull</t>
+  </si>
+  <si>
+    <t>Chroicocephalus philadelphia</t>
+  </si>
+  <si>
+    <t>Gull-billed Tern</t>
+  </si>
+  <si>
+    <t>Gelochelidon nilotica</t>
+  </si>
+  <si>
+    <t>Caspian Tern</t>
+  </si>
+  <si>
+    <t>Hydroprogne caspia</t>
+  </si>
+  <si>
+    <t>Royal Tern</t>
+  </si>
+  <si>
+    <t>Thalasseus maximus</t>
+  </si>
+  <si>
+    <t>Cabot's Tern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalasseus acuflavidus </t>
+  </si>
+  <si>
+    <t>Forster's Tern</t>
+  </si>
+  <si>
+    <t>Sterna forsteri</t>
+  </si>
+  <si>
+    <t>Common Tern</t>
+  </si>
+  <si>
+    <t>Sterna hirundo</t>
+  </si>
+  <si>
+    <t>Little Tern</t>
+  </si>
+  <si>
+    <t>Sterna albifrons</t>
+  </si>
+  <si>
+    <t>Black Tern</t>
+  </si>
+  <si>
+    <t>Chlidonias niger</t>
+  </si>
+  <si>
+    <t>Black Skimmer</t>
+  </si>
+  <si>
+    <t>Rynchops niger</t>
+  </si>
+  <si>
+    <t>Sooty Shearwater</t>
+  </si>
+  <si>
+    <t>Puffinus griseus</t>
+  </si>
+  <si>
+    <t>Mallard</t>
+  </si>
+  <si>
+    <t>Anas platyrhnchos</t>
+  </si>
+  <si>
+    <t>American Black Duck</t>
+  </si>
+  <si>
+    <t>Anas rubripes rubripes</t>
+  </si>
+  <si>
+    <t>Anatidae</t>
+  </si>
+  <si>
+    <t>Gadwall</t>
+  </si>
+  <si>
+    <t>Anas strepera</t>
+  </si>
+  <si>
+    <t>Baldpate</t>
+  </si>
+  <si>
+    <t>Mareca americana</t>
+  </si>
+  <si>
+    <t>Green-winged Teal</t>
+  </si>
+  <si>
+    <t>Anas carolinensis</t>
+  </si>
+  <si>
+    <t>Blue-winged Teal</t>
+  </si>
+  <si>
+    <t>Spatula discors</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Arthropoda</t>
+  </si>
+  <si>
+    <t>Insecta</t>
+  </si>
+  <si>
+    <t>Malacostraca</t>
+  </si>
+  <si>
+    <t>Decapoda</t>
+  </si>
+  <si>
+    <t>Chordata</t>
   </si>
 </sst>
 </file>
@@ -485,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +811,369 @@
       <c r="K2" t="s">
         <v>47</v>
       </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>95</v>
+      </c>
+      <c r="U2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>95</v>
+      </c>
+      <c r="U4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
resolved small merge conflict in dietdatabase
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_Howell_1924_GN.xlsx
+++ b/AvianDietDatabase_Howell_1924_GN.xlsx
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finished with Passmore 1981, deleted related records from repo after putting them into the dietdatabase
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_Howell_1924_GN.xlsx
+++ b/AvianDietDatabase_Howell_1924_GN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="100">
   <si>
     <t>Common_Name</t>
   </si>
@@ -155,178 +155,175 @@
     <t>eBird Clements Checklist v2018</t>
   </si>
   <si>
-    <t>Horned Grebe</t>
-  </si>
-  <si>
-    <t>Podiceps auritus</t>
-  </si>
-  <si>
-    <t>Podicipedidae</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>Alabama</t>
   </si>
   <si>
-    <t>Pied-billed Grebe</t>
-  </si>
-  <si>
-    <t>Podilymbus podiceps</t>
-  </si>
-  <si>
-    <t>Common Loon</t>
-  </si>
-  <si>
-    <t>Gavia immer</t>
-  </si>
-  <si>
-    <t>Gaviidae</t>
-  </si>
-  <si>
-    <t>European Herring Gull</t>
-  </si>
-  <si>
-    <t>Larus argentatus</t>
-  </si>
-  <si>
     <t>Laridae</t>
   </si>
   <si>
-    <t>Ring-billed Gull</t>
-  </si>
-  <si>
-    <t>Larus delawarensis</t>
-  </si>
-  <si>
-    <t>Laughing Gull</t>
-  </si>
-  <si>
-    <t>Leucophaeus atricilla</t>
-  </si>
-  <si>
-    <t>Bonaparte's Gull</t>
-  </si>
-  <si>
-    <t>Chroicocephalus philadelphia</t>
-  </si>
-  <si>
-    <t>Gull-billed Tern</t>
-  </si>
-  <si>
-    <t>Gelochelidon nilotica</t>
-  </si>
-  <si>
-    <t>Caspian Tern</t>
-  </si>
-  <si>
-    <t>Hydroprogne caspia</t>
-  </si>
-  <si>
     <t>Royal Tern</t>
   </si>
   <si>
     <t>Thalasseus maximus</t>
   </si>
   <si>
-    <t>Cabot's Tern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thalasseus acuflavidus </t>
-  </si>
-  <si>
-    <t>Forster's Tern</t>
-  </si>
-  <si>
-    <t>Sterna forsteri</t>
-  </si>
-  <si>
-    <t>Common Tern</t>
-  </si>
-  <si>
-    <t>Sterna hirundo</t>
-  </si>
-  <si>
-    <t>Little Tern</t>
-  </si>
-  <si>
-    <t>Sterna albifrons</t>
-  </si>
-  <si>
-    <t>Black Tern</t>
-  </si>
-  <si>
-    <t>Chlidonias niger</t>
-  </si>
-  <si>
-    <t>Black Skimmer</t>
-  </si>
-  <si>
-    <t>Rynchops niger</t>
-  </si>
-  <si>
-    <t>Sooty Shearwater</t>
-  </si>
-  <si>
-    <t>Puffinus griseus</t>
-  </si>
-  <si>
     <t>Mallard</t>
   </si>
   <si>
     <t>Anas platyrhnchos</t>
   </si>
   <si>
-    <t>American Black Duck</t>
-  </si>
-  <si>
-    <t>Anas rubripes rubripes</t>
-  </si>
-  <si>
     <t>Anatidae</t>
   </si>
   <si>
     <t>Gadwall</t>
   </si>
   <si>
-    <t>Anas strepera</t>
-  </si>
-  <si>
-    <t>Baldpate</t>
-  </si>
-  <si>
     <t>Mareca americana</t>
   </si>
   <si>
-    <t>Green-winged Teal</t>
-  </si>
-  <si>
-    <t>Anas carolinensis</t>
-  </si>
-  <si>
-    <t>Blue-winged Teal</t>
-  </si>
-  <si>
-    <t>Spatula discors</t>
-  </si>
-  <si>
     <t>Animalia</t>
   </si>
   <si>
     <t>Arthropoda</t>
   </si>
   <si>
-    <t>Insecta</t>
-  </si>
-  <si>
     <t>Malacostraca</t>
   </si>
   <si>
-    <t>Decapoda</t>
-  </si>
-  <si>
     <t>Chordata</t>
+  </si>
+  <si>
+    <t>wt_or_vol</t>
+  </si>
+  <si>
+    <t>Teleostei</t>
+  </si>
+  <si>
+    <t>Clupeiformes</t>
+  </si>
+  <si>
+    <t>Clupeoidei</t>
+  </si>
+  <si>
+    <t>Clupeidae</t>
+  </si>
+  <si>
+    <t>Actinopterygii</t>
+  </si>
+  <si>
+    <t>Perciformes</t>
+  </si>
+  <si>
+    <t>Percidae</t>
+  </si>
+  <si>
+    <t>Double-crested Cormorant</t>
+  </si>
+  <si>
+    <t>Phalacrocorax auritus</t>
+  </si>
+  <si>
+    <t>Phalacrocoracidae</t>
+  </si>
+  <si>
+    <t>Dorosoma</t>
+  </si>
+  <si>
+    <t>Dorosoma cepedianum</t>
+  </si>
+  <si>
+    <t>Occurrence</t>
+  </si>
+  <si>
+    <t>Anguilliformes</t>
+  </si>
+  <si>
+    <t>Howell, A. 1928. Birds of Alabama. Department of Game and Fisheries of Alabama.</t>
+  </si>
+  <si>
+    <t>Plantae</t>
+  </si>
+  <si>
+    <t>Magnoliopsida</t>
+  </si>
+  <si>
+    <t>Poales</t>
+  </si>
+  <si>
+    <t>Cyperaceae</t>
+  </si>
+  <si>
+    <t>Carex</t>
+  </si>
+  <si>
+    <t>Tracheophyta</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2019</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2020</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2021</t>
+  </si>
+  <si>
+    <t>Poaceae</t>
+  </si>
+  <si>
+    <t>Fagales</t>
+  </si>
+  <si>
+    <t>Fagaceae</t>
+  </si>
+  <si>
+    <t>Quercus</t>
+  </si>
+  <si>
+    <t>seed</t>
+  </si>
+  <si>
+    <t>Mollusca</t>
+  </si>
+  <si>
+    <t>Mareca strepera</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2022</t>
+  </si>
+  <si>
+    <t>American Wigeon</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2023</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2024</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2025</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2026</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2027</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2028</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2029</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2030</t>
+  </si>
+  <si>
+    <t>eBird Clements Checklist v2031</t>
   </si>
 </sst>
 </file>
@@ -644,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP26"/>
+  <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,10 +779,10 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -793,386 +790,1141 @@
       <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH2">
+        <v>0.03</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W3" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH3">
+        <v>0.65</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>95</v>
-      </c>
-      <c r="U2" t="s">
-        <v>96</v>
-      </c>
-      <c r="V2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK2">
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W4" t="s">
+        <v>63</v>
+      </c>
+      <c r="X4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH4">
+        <v>0.32</v>
+      </c>
+      <c r="AI4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="T3" t="s">
-        <v>95</v>
-      </c>
-      <c r="U3" t="s">
-        <v>96</v>
-      </c>
-      <c r="V3" t="s">
-        <v>98</v>
-      </c>
-      <c r="W3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="T4" t="s">
-        <v>95</v>
-      </c>
-      <c r="U4" t="s">
-        <v>100</v>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ5">
+        <v>3</v>
+      </c>
+      <c r="AK5">
+        <v>2</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
       </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U6" t="s">
+        <v>56</v>
+      </c>
+      <c r="V6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W6" t="s">
+        <v>71</v>
+      </c>
+      <c r="X6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH6">
+        <v>0.5</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ6">
+        <v>3</v>
+      </c>
+      <c r="AK6">
+        <v>2</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
         <v>42</v>
       </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" t="s">
+        <v>78</v>
+      </c>
+      <c r="V7" t="s">
+        <v>74</v>
+      </c>
+      <c r="W7" t="s">
+        <v>75</v>
+      </c>
+      <c r="X7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH7">
+        <v>0.216</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK7">
+        <v>1578</v>
+      </c>
+      <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>73</v>
+      </c>
+      <c r="U8" t="s">
+        <v>78</v>
+      </c>
+      <c r="V8" t="s">
+        <v>74</v>
+      </c>
+      <c r="W8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH8">
+        <v>0.13</v>
+      </c>
+      <c r="AI8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
+      <c r="AJ8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK8">
+        <v>1578</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>73</v>
+      </c>
+      <c r="U9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V9" t="s">
+        <v>74</v>
+      </c>
+      <c r="W9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH9">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK9">
+        <v>1578</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>81</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH10">
+        <v>0.1</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK10">
+        <v>1578</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>89</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH11">
+        <v>0.42</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>89</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" t="s">
+        <v>44</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH13">
+        <v>0.02</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL13">
+        <v>1</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>91</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH14">
+        <v>6.7699999999999996E-2</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL14">
+        <v>1</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>92</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH15">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL15">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH16">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH17">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL17">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH18">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL18">
+        <v>1</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH19">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH20">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
+        <v>99</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH22">
+        <v>1.47E-2</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>